<commit_message>
first committ jun 27
</commit_message>
<xml_diff>
--- a/new.xlsx
+++ b/new.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5367" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5419" uniqueCount="71">
   <si>
     <t>stock</t>
   </si>
@@ -300,7 +300,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10710">
+  <cellXfs count="10812">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="176" xfId="5">
       <alignment wrapText="1"/>
@@ -32427,6 +32427,312 @@
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -32742,410 +33048,410 @@
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="10608" t="s">
+      <c r="A1" s="10710" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10609" t="s">
+      <c r="B1" s="10711" t="s">
         <v>1</v>
       </c>
     </row>
     <row ht="54" r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="10610" t="s">
+      <c r="A2" s="10712" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="10660" t="n">
+      <c r="B2" s="10762" t="n">
         <v>3.04</v>
       </c>
     </row>
     <row ht="40.5" r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="10611" t="s">
+      <c r="A3" s="10713" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="10661" t="n">
+      <c r="B3" s="10763" t="n">
         <v>1.11</v>
       </c>
     </row>
     <row ht="27" r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="10612" t="s">
+      <c r="A4" s="10714" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="10662" t="n">
+      <c r="B4" s="10764" t="n">
         <v>2.71</v>
       </c>
     </row>
     <row ht="27" r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="10613" t="s">
+      <c r="A5" s="10715" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="10663" t="n">
+      <c r="B5" s="10765" t="n">
         <v>2.4</v>
       </c>
     </row>
     <row ht="40.5" r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="10614" t="s">
+      <c r="A6" s="10716" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10664" t="n">
+      <c r="B6" s="10766" t="n">
         <v>1.21</v>
       </c>
     </row>
     <row ht="67.5" r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="10615" t="s">
+      <c r="A7" s="10717" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="10665" t="n">
+      <c r="B7" s="10767" t="n">
         <v>5.4</v>
       </c>
     </row>
     <row ht="27" r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" s="10616" t="s">
+      <c r="A8" s="10718" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="10666" t="n">
+      <c r="B8" s="10768" t="n">
         <v>1.9</v>
       </c>
     </row>
     <row ht="54" r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" s="10617" t="s">
+      <c r="A9" s="10719" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="10667" t="n">
+      <c r="B9" s="10769" t="n">
         <v>1.1</v>
       </c>
     </row>
     <row ht="27" r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" s="10618" t="s">
+      <c r="A10" s="10720" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="10668" t="n">
+      <c r="B10" s="10770" t="n">
         <v>0.77</v>
       </c>
     </row>
     <row ht="40.5" r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" s="10619" t="s">
+      <c r="A11" s="10721" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="10669" t="n">
+      <c r="B11" s="10771" t="n">
         <v>3.02</v>
       </c>
     </row>
     <row ht="81" r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" s="10620" t="s">
+      <c r="A12" s="10722" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="10670" t="n">
+      <c r="B12" s="10772" t="n">
         <v>1.36</v>
       </c>
     </row>
     <row ht="27" r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" s="10621" t="s">
+      <c r="A13" s="10723" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="10671" t="n">
+      <c r="B13" s="10773" t="n">
         <v>5.22</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" s="10622" t="s">
+      <c r="A14" s="10724" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="10672" t="n">
+      <c r="B14" s="10774" t="n">
         <v>0.36</v>
       </c>
     </row>
     <row ht="40.5" r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" s="10623" t="s">
+      <c r="A15" s="10725" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="10673" t="n">
+      <c r="B15" s="10775" t="n">
         <v>2.75</v>
       </c>
     </row>
     <row ht="67.5" r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" s="10624" t="s">
+      <c r="A16" s="10726" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="10674" t="n">
+      <c r="B16" s="10776" t="n">
         <v>3.43</v>
       </c>
     </row>
     <row ht="40.5" r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" s="10625" t="s">
+      <c r="A17" s="10727" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="10675" t="n">
+      <c r="B17" s="10777" t="n">
         <v>0.69</v>
       </c>
     </row>
     <row ht="40.5" r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" s="10626" t="s">
+      <c r="A18" s="10728" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="10676" t="n">
+      <c r="B18" s="10778" t="n">
         <v>1.42</v>
       </c>
     </row>
     <row ht="27" r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" s="10627" t="s">
+      <c r="A19" s="10729" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="10677" t="n">
+      <c r="B19" s="10779" t="n">
         <v>0.69</v>
       </c>
     </row>
     <row ht="67.5" r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" s="10628" t="s">
+      <c r="A20" s="10730" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="10678" t="n">
+      <c r="B20" s="10780" t="n">
         <v>0.42</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" s="10629" t="s">
+      <c r="A21" s="10731" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="10679" t="n">
+      <c r="B21" s="10781" t="n">
         <v>1.42</v>
       </c>
     </row>
     <row ht="27" r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" s="10630" t="s">
+      <c r="A22" s="10732" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="10680" t="n">
+      <c r="B22" s="10782" t="n">
         <v>0.77</v>
       </c>
     </row>
     <row ht="54" r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" s="10631" t="s">
+      <c r="A23" s="10733" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="10681" t="n">
+      <c r="B23" s="10783" t="n">
         <v>0.54</v>
       </c>
     </row>
     <row ht="27" r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24" s="10632" t="s">
+      <c r="A24" s="10734" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="10682" t="n">
+      <c r="B24" s="10784" t="n">
         <v>3.16</v>
       </c>
     </row>
     <row ht="67.5" r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" s="10633" t="s">
+      <c r="A25" s="10735" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="10683" t="n">
+      <c r="B25" s="10785" t="n">
         <v>1.62</v>
       </c>
     </row>
     <row ht="40.5" r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" s="10634" t="s">
+      <c r="A26" s="10736" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="10684" t="n">
+      <c r="B26" s="10786" t="n">
         <v>1.38</v>
       </c>
     </row>
     <row ht="81" r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" s="10635" t="s">
+      <c r="A27" s="10737" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="10685" t="n">
+      <c r="B27" s="10787" t="n">
         <v>2.05</v>
       </c>
     </row>
     <row ht="54" r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="10636" t="s">
+      <c r="A28" s="10738" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="10686" t="n">
+      <c r="B28" s="10788" t="n">
         <v>10.72</v>
       </c>
     </row>
     <row ht="40.5" r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="10637" t="s">
+      <c r="A29" s="10739" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="10687" t="n">
+      <c r="B29" s="10789" t="n">
         <v>1.37</v>
       </c>
     </row>
     <row ht="54" r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="10638" t="s">
+      <c r="A30" s="10740" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="10688" t="n">
+      <c r="B30" s="10790" t="n">
         <v>1.29</v>
       </c>
     </row>
     <row ht="40.5" r="31" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A31" s="10639" t="s">
+      <c r="A31" s="10741" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="10689" t="n">
+      <c r="B31" s="10791" t="n">
         <v>0.98</v>
       </c>
     </row>
     <row ht="40.5" r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32" s="10640" t="s">
+      <c r="A32" s="10742" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="10690" t="n">
+      <c r="B32" s="10792" t="n">
         <v>1.06</v>
       </c>
     </row>
     <row ht="27" r="33" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A33" s="10641" t="s">
+      <c r="A33" s="10743" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="10691" t="n">
+      <c r="B33" s="10793" t="n">
         <v>1.39</v>
       </c>
     </row>
     <row ht="67.5" r="34" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A34" s="10642" t="s">
+      <c r="A34" s="10744" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="10692" t="n">
+      <c r="B34" s="10794" t="n">
         <v>6.14</v>
       </c>
     </row>
     <row ht="54" r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35" s="10643" t="s">
+      <c r="A35" s="10745" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="10693" t="n">
+      <c r="B35" s="10795" t="n">
         <v>0.36</v>
       </c>
     </row>
     <row ht="54" r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36" s="10644" t="s">
+      <c r="A36" s="10746" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="10694" t="n">
+      <c r="B36" s="10796" t="n">
         <v>1.78</v>
       </c>
     </row>
     <row ht="40.5" r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37" s="10645" t="s">
+      <c r="A37" s="10747" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="10695" t="n">
+      <c r="B37" s="10797" t="n">
         <v>1.04</v>
       </c>
     </row>
     <row ht="54" r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" s="10646" t="s">
+      <c r="A38" s="10748" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="10696" t="n">
+      <c r="B38" s="10798" t="n">
         <v>0.26</v>
       </c>
     </row>
     <row ht="40.5" r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39" s="10647" t="s">
+      <c r="A39" s="10749" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="10697" t="n">
+      <c r="B39" s="10799" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row ht="54" r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40" s="10648" t="s">
+      <c r="A40" s="10750" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="10698" t="n">
+      <c r="B40" s="10800" t="n">
         <v>0.39</v>
       </c>
     </row>
     <row ht="54" r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41" s="10649" t="s">
+      <c r="A41" s="10751" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="10699" t="n">
+      <c r="B41" s="10801" t="n">
         <v>4.24</v>
       </c>
     </row>
     <row ht="54" r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42" s="10650" t="s">
+      <c r="A42" s="10752" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="10700" t="n">
+      <c r="B42" s="10802" t="n">
         <v>4.62</v>
       </c>
     </row>
     <row ht="40.5" r="43" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A43" s="10651" t="s">
+      <c r="A43" s="10753" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="10701" t="n">
+      <c r="B43" s="10803" t="n">
         <v>1.61</v>
       </c>
     </row>
     <row ht="40.5" r="44" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A44" s="10652" t="s">
+      <c r="A44" s="10754" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="10702" t="n">
+      <c r="B44" s="10804" t="n">
         <v>0.77</v>
       </c>
     </row>
     <row ht="54" r="45" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A45" s="10653" t="s">
+      <c r="A45" s="10755" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="10703" t="n">
+      <c r="B45" s="10805" t="n">
         <v>0.75</v>
       </c>
     </row>
     <row ht="81" r="46" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A46" s="10654" t="s">
+      <c r="A46" s="10756" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="10704" t="n">
+      <c r="B46" s="10806" t="n">
         <v>2.22</v>
       </c>
     </row>
     <row ht="27" r="47" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A47" s="10655" t="s">
+      <c r="A47" s="10757" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="10705" t="n">
+      <c r="B47" s="10807" t="n">
         <v>2.27</v>
       </c>
     </row>
     <row ht="54" r="48" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A48" s="10656" t="s">
+      <c r="A48" s="10758" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="10706" t="n">
+      <c r="B48" s="10808" t="n">
         <v>1.99</v>
       </c>
     </row>
     <row ht="40.5" r="49" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A49" s="10657" t="s">
+      <c r="A49" s="10759" t="s">
         <v>46</v>
       </c>
-      <c r="B49" s="10707" t="n">
+      <c r="B49" s="10809" t="n">
         <v>1.75</v>
       </c>
     </row>
     <row ht="54" r="50" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A50" s="10658" t="s">
+      <c r="A50" s="10760" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="10708" t="n">
+      <c r="B50" s="10810" t="n">
         <v>1.41</v>
       </c>
     </row>
     <row ht="67.5" r="51" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A51" s="10659" t="s">
+      <c r="A51" s="10761" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="10709" t="n">
+      <c r="B51" s="10811" t="n">
         <v>1.13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
628 morning first comit
</commit_message>
<xml_diff>
--- a/new.xlsx
+++ b/new.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5627" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5731" uniqueCount="74">
   <si>
     <t>stock</t>
   </si>
@@ -309,7 +309,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11220">
+  <cellXfs count="11424">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="176" xfId="5">
       <alignment wrapText="1"/>
@@ -20454,6 +20454,618 @@
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="176" xfId="5">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
@@ -34281,411 +34893,411 @@
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="11118" t="s">
+      <c r="A1" s="11322" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11119" t="s">
+      <c r="B1" s="11323" t="s">
         <v>1</v>
       </c>
     </row>
     <row ht="54" r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="11120" t="s">
+      <c r="A2" s="11324" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11170" t="n">
-        <v>2.89</v>
+      <c r="B2" s="11374" t="n">
+        <v>2.86</v>
       </c>
     </row>
     <row ht="40.5" r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="11121" t="s">
+      <c r="A3" s="11325" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="11171" t="n">
-        <v>1.95</v>
+      <c r="B3" s="11375" t="n">
+        <v>1.96</v>
       </c>
     </row>
     <row ht="27" r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="11122" t="s">
+      <c r="A4" s="11326" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="11172" t="n">
-        <v>2.59</v>
+      <c r="B4" s="11376" t="n">
+        <v>2.56</v>
       </c>
     </row>
     <row ht="27" r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="11123" t="s">
+      <c r="A5" s="11327" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="11173" t="n">
+      <c r="B5" s="11377" t="n">
         <v>2.27</v>
       </c>
     </row>
     <row ht="40.5" r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="11124" t="s">
+      <c r="A6" s="11328" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="11174" t="n">
-        <v>1.34</v>
+      <c r="B6" s="11378" t="n">
+        <v>1.33</v>
       </c>
     </row>
     <row ht="67.5" r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="11125" t="s">
+      <c r="A7" s="11329" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="11175" t="n">
-        <v>5.27</v>
+      <c r="B7" s="11379" t="n">
+        <v>5.26</v>
       </c>
     </row>
     <row ht="27" r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" s="11126" t="s">
+      <c r="A8" s="11330" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="11176" t="n">
-        <v>1.81</v>
+      <c r="B8" s="11380" t="n">
+        <v>1.79</v>
       </c>
     </row>
     <row ht="54" r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" s="11127" t="s">
+      <c r="A9" s="11331" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="11177" t="n">
+      <c r="B9" s="11381" t="n">
         <v>1.05</v>
       </c>
     </row>
     <row ht="27" r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" s="11128" t="s">
+      <c r="A10" s="11332" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="11178" t="n">
-        <v>1.41</v>
+      <c r="B10" s="11382" t="n">
+        <v>1.43</v>
       </c>
     </row>
     <row ht="40.5" r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" s="11129" t="s">
+      <c r="A11" s="11333" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="11179" t="n">
-        <v>2.88</v>
+      <c r="B11" s="11383" t="n">
+        <v>2.83</v>
       </c>
     </row>
     <row ht="81" r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" s="11130" t="s">
+      <c r="A12" s="11334" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="11180" t="n">
+      <c r="B12" s="11384" t="n">
         <v>1.04</v>
       </c>
     </row>
     <row ht="27" r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" s="11131" t="s">
+      <c r="A13" s="11335" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="11181" t="n">
-        <v>0.89</v>
+      <c r="B13" s="11385" t="n">
+        <v>0.9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" s="11132" t="s">
+      <c r="A14" s="11336" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="11182" t="n">
-        <v>0.36</v>
+      <c r="B14" s="11386" t="n">
+        <v>0.35</v>
       </c>
     </row>
     <row ht="40.5" r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" s="11133" t="s">
+      <c r="A15" s="11337" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="11183" t="n">
-        <v>1.03</v>
+      <c r="B15" s="11387" t="n">
+        <v>1.02</v>
       </c>
     </row>
     <row ht="67.5" r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" s="11134" t="s">
+      <c r="A16" s="11338" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="11184" t="n">
-        <v>4.88</v>
+      <c r="B16" s="11388" t="n">
+        <v>4.97</v>
       </c>
     </row>
     <row ht="40.5" r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" s="11135" t="s">
+      <c r="A17" s="11339" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="11185" t="n">
-        <v>0.79</v>
+      <c r="B17" s="11389" t="n">
+        <v>0.8</v>
       </c>
     </row>
     <row ht="40.5" r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" s="11136" t="s">
+      <c r="A18" s="11340" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="11186" t="n">
-        <v>1.28</v>
+      <c r="B18" s="11390" t="n">
+        <v>1.27</v>
       </c>
     </row>
     <row ht="27" r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" s="11137" t="s">
+      <c r="A19" s="11341" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="11187" t="n">
-        <v>3.67</v>
+      <c r="B19" s="11391" t="n">
+        <v>3.62</v>
       </c>
     </row>
     <row ht="67.5" r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" s="11138" t="s">
+      <c r="A20" s="11342" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="11188" t="n">
-        <v>1.95</v>
+      <c r="B20" s="11392" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" s="11139" t="s">
+      <c r="A21" s="11343" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="11189" t="n">
-        <v>2.69</v>
+      <c r="B21" s="11393" t="n">
+        <v>2.72</v>
       </c>
     </row>
     <row ht="27" r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" s="11140" t="s">
+      <c r="A22" s="11344" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="11190" t="n">
-        <v>0.68</v>
+      <c r="B22" s="11394" t="n">
+        <v>0.67</v>
       </c>
     </row>
     <row ht="54" r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" s="11141" t="s">
+      <c r="A23" s="11345" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="11191" t="n">
-        <v>0.64</v>
+      <c r="B23" s="11395" t="n">
+        <v>0.65</v>
       </c>
     </row>
     <row ht="27" r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24" s="11142" t="s">
+      <c r="A24" s="11346" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="11192" t="n">
-        <v>1.33</v>
+      <c r="B24" s="11396" t="n">
+        <v>1.32</v>
       </c>
     </row>
     <row ht="67.5" r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" s="11143" t="s">
+      <c r="A25" s="11347" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="11193" t="n">
+      <c r="B25" s="11397" t="n">
         <v>0.73</v>
       </c>
     </row>
     <row ht="40.5" r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" s="11144" t="s">
+      <c r="A26" s="11348" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="11194" t="n">
+      <c r="B26" s="11398" t="n">
         <v>0.39</v>
       </c>
     </row>
     <row ht="81" r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" s="11145" t="s">
+      <c r="A27" s="11349" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="11195" t="n">
-        <v>1.38</v>
+      <c r="B27" s="11399" t="n">
+        <v>1.37</v>
       </c>
     </row>
     <row ht="54" r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="11146" t="s">
+      <c r="A28" s="11350" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="11196" t="n">
+      <c r="B28" s="11400" t="n">
         <v>1.56</v>
       </c>
     </row>
     <row ht="40.5" r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="11147" t="s">
+      <c r="A29" s="11351" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="11197" t="n">
+      <c r="B29" s="11401" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row ht="54" r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="11148" t="s">
+      <c r="A30" s="11352" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="11198" t="n">
-        <v>3.07</v>
+      <c r="B30" s="11402" t="n">
+        <v>3.11</v>
       </c>
     </row>
     <row ht="40.5" r="31" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A31" s="11149" t="s">
+      <c r="A31" s="11353" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="11199" t="n">
-        <v>10.68</v>
+      <c r="B31" s="11403" t="n">
+        <v>10.61</v>
       </c>
     </row>
     <row ht="40.5" r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32" s="11150" t="s">
+      <c r="A32" s="11354" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="11200" t="n">
-        <v>1.33</v>
+      <c r="B32" s="11404" t="n">
+        <v>1.32</v>
       </c>
     </row>
     <row ht="27" r="33" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A33" s="11151" t="s">
+      <c r="A33" s="11355" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="11201" t="n">
+      <c r="B33" s="11405" t="n">
         <v>1.93</v>
       </c>
     </row>
     <row ht="67.5" r="34" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A34" s="11152" t="s">
+      <c r="A34" s="11356" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="11202" t="n">
-        <v>1.3</v>
+      <c r="B34" s="11406" t="n">
+        <v>1.29</v>
       </c>
     </row>
     <row ht="54" r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35" s="11153" t="s">
+      <c r="A35" s="11357" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="11203" t="n">
-        <v>1.26</v>
+      <c r="B35" s="11407" t="n">
+        <v>1.24</v>
       </c>
     </row>
     <row ht="54" r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36" s="11154" t="s">
+      <c r="A36" s="11358" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="11204" t="n">
-        <v>1.36</v>
+      <c r="B36" s="11408" t="n">
+        <v>1.39</v>
       </c>
     </row>
     <row ht="40.5" r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37" s="11155" t="s">
+      <c r="A37" s="11359" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="11205" t="n">
-        <v>0.94</v>
+      <c r="B37" s="11409" t="n">
+        <v>0.93</v>
       </c>
     </row>
     <row ht="54" r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" s="11156" t="s">
+      <c r="A38" s="11360" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="11206" t="n">
-        <v>1.0</v>
+      <c r="B38" s="11410" t="n">
+        <v>1.01</v>
       </c>
     </row>
     <row ht="40.5" r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39" s="11157" t="s">
+      <c r="A39" s="11361" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="11207" t="n">
-        <v>1.67</v>
+      <c r="B39" s="11411" t="n">
+        <v>1.7</v>
       </c>
     </row>
     <row ht="54" r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40" s="11158" t="s">
+      <c r="A40" s="11362" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="11208" t="n">
-        <v>6.32</v>
+      <c r="B40" s="11412" t="n">
+        <v>6.28</v>
       </c>
     </row>
     <row ht="54" r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41" s="11159" t="s">
+      <c r="A41" s="11363" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="11209" t="n">
+      <c r="B41" s="11413" t="n">
         <v>0.34</v>
       </c>
     </row>
     <row ht="54" r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42" s="11160" t="s">
+      <c r="A42" s="11364" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="11210" t="n">
+      <c r="B42" s="11414" t="n">
         <v>0.44</v>
       </c>
     </row>
     <row ht="40.5" r="43" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A43" s="11161" t="s">
+      <c r="A43" s="11365" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="11211" t="n">
-        <v>1.01</v>
+      <c r="B43" s="11415" t="n">
+        <v>1.05</v>
       </c>
     </row>
     <row ht="40.5" r="44" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A44" s="11162" t="s">
+      <c r="A44" s="11366" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="11212" t="n">
-        <v>1.54</v>
+      <c r="B44" s="11416" t="n">
+        <v>1.57</v>
       </c>
     </row>
     <row ht="54" r="45" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A45" s="11163" t="s">
+      <c r="A45" s="11367" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="11213" t="n">
-        <v>4.06</v>
+      <c r="B45" s="11417" t="n">
+        <v>4.04</v>
       </c>
     </row>
     <row ht="81" r="46" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A46" s="11164" t="s">
+      <c r="A46" s="11368" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="11214" t="n">
+      <c r="B46" s="11418" t="n">
         <v>2.07</v>
       </c>
     </row>
     <row ht="27" r="47" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A47" s="11165" t="s">
+      <c r="A47" s="11369" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="11215" t="n">
-        <v>2.21</v>
+      <c r="B47" s="11419" t="n">
+        <v>2.26</v>
       </c>
     </row>
     <row ht="54" r="48" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A48" s="11166" t="s">
+      <c r="A48" s="11370" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="11216" t="n">
-        <v>4.36</v>
+      <c r="B48" s="11420" t="n">
+        <v>4.34</v>
       </c>
     </row>
     <row ht="40.5" r="49" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A49" s="11167" t="s">
+      <c r="A49" s="11371" t="s">
         <v>46</v>
       </c>
-      <c r="B49" s="11217" t="n">
-        <v>2.05</v>
+      <c r="B49" s="11421" t="n">
+        <v>2.06</v>
       </c>
     </row>
     <row ht="54" r="50" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A50" s="11168" t="s">
+      <c r="A50" s="11372" t="s">
         <v>42</v>
       </c>
-      <c r="B50" s="11218" t="n">
-        <v>0.72</v>
+      <c r="B50" s="11422" t="n">
+        <v>0.71</v>
       </c>
     </row>
     <row ht="67.5" r="51" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A51" s="11169" t="s">
+      <c r="A51" s="11373" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="11219" t="n">
-        <v>1.09</v>
+      <c r="B51" s="11423" t="n">
+        <v>1.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first comit jun 29
</commit_message>
<xml_diff>
--- a/new.xlsx
+++ b/new.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5731" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5783" uniqueCount="74">
   <si>
     <t>stock</t>
   </si>
@@ -309,7 +309,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11424">
+  <cellXfs count="11526">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="176" xfId="5">
       <alignment wrapText="1"/>
@@ -20454,6 +20454,312 @@
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="176" xfId="5">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
@@ -34893,411 +35199,411 @@
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="11322" t="s">
+      <c r="A1" s="11424" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11323" t="s">
+      <c r="B1" s="11425" t="s">
         <v>1</v>
       </c>
     </row>
     <row ht="54" r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="11324" t="s">
+      <c r="A2" s="11426" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11374" t="n">
-        <v>2.86</v>
+      <c r="B2" s="11476" t="n">
+        <v>2.84</v>
       </c>
     </row>
     <row ht="40.5" r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="11325" t="s">
+      <c r="A3" s="11427" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="11375" t="n">
+      <c r="B3" s="11477" t="n">
         <v>1.96</v>
       </c>
     </row>
     <row ht="27" r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="11326" t="s">
+      <c r="A4" s="11428" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="11376" t="n">
-        <v>2.56</v>
+      <c r="B4" s="11478" t="n">
+        <v>2.53</v>
       </c>
     </row>
     <row ht="27" r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="11327" t="s">
+      <c r="A5" s="11429" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="11377" t="n">
-        <v>2.27</v>
+      <c r="B5" s="11479" t="n">
+        <v>2.26</v>
       </c>
     </row>
     <row ht="40.5" r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="11328" t="s">
+      <c r="A6" s="11430" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="11378" t="n">
-        <v>1.33</v>
+      <c r="B6" s="11480" t="n">
+        <v>1.3</v>
       </c>
     </row>
     <row ht="67.5" r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="11329" t="s">
+      <c r="A7" s="11431" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="11379" t="n">
-        <v>5.26</v>
+      <c r="B7" s="11481" t="n">
+        <v>5.27</v>
       </c>
     </row>
     <row ht="27" r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" s="11330" t="s">
+      <c r="A8" s="11432" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="11380" t="n">
-        <v>1.79</v>
+      <c r="B8" s="11482" t="n">
+        <v>1.78</v>
       </c>
     </row>
     <row ht="54" r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" s="11331" t="s">
+      <c r="A9" s="11433" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="11381" t="n">
-        <v>1.05</v>
+      <c r="B9" s="11483" t="n">
+        <v>1.07</v>
       </c>
     </row>
     <row ht="27" r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" s="11332" t="s">
+      <c r="A10" s="11434" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="11382" t="n">
-        <v>1.43</v>
+      <c r="B10" s="11484" t="n">
+        <v>1.42</v>
       </c>
     </row>
     <row ht="40.5" r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" s="11333" t="s">
+      <c r="A11" s="11435" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="11383" t="n">
-        <v>2.83</v>
+      <c r="B11" s="11485" t="n">
+        <v>2.82</v>
       </c>
     </row>
     <row ht="81" r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" s="11334" t="s">
+      <c r="A12" s="11436" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="11384" t="n">
+      <c r="B12" s="11486" t="n">
         <v>1.04</v>
       </c>
     </row>
     <row ht="27" r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" s="11335" t="s">
+      <c r="A13" s="11437" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="11385" t="n">
+      <c r="B13" s="11487" t="n">
         <v>0.9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" s="11336" t="s">
+      <c r="A14" s="11438" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="11386" t="n">
-        <v>0.35</v>
+      <c r="B14" s="11488" t="n">
+        <v>0.36</v>
       </c>
     </row>
     <row ht="40.5" r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" s="11337" t="s">
+      <c r="A15" s="11439" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="11387" t="n">
+      <c r="B15" s="11489" t="n">
         <v>1.02</v>
       </c>
     </row>
     <row ht="67.5" r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" s="11338" t="s">
+      <c r="A16" s="11440" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="11388" t="n">
-        <v>4.97</v>
+      <c r="B16" s="11490" t="n">
+        <v>4.94</v>
       </c>
     </row>
     <row ht="40.5" r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" s="11339" t="s">
+      <c r="A17" s="11441" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="11389" t="n">
+      <c r="B17" s="11491" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row ht="40.5" r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" s="11340" t="s">
+      <c r="A18" s="11442" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="11390" t="n">
-        <v>1.27</v>
+      <c r="B18" s="11492" t="n">
+        <v>1.26</v>
       </c>
     </row>
     <row ht="27" r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" s="11341" t="s">
+      <c r="A19" s="11443" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="11391" t="n">
-        <v>3.62</v>
+      <c r="B19" s="11493" t="n">
+        <v>3.59</v>
       </c>
     </row>
     <row ht="67.5" r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" s="11342" t="s">
+      <c r="A20" s="11444" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="11392" t="n">
-        <v>2.0</v>
+      <c r="B20" s="11494" t="n">
+        <v>1.98</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" s="11343" t="s">
+      <c r="A21" s="11445" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="11393" t="n">
-        <v>2.72</v>
+      <c r="B21" s="11495" t="n">
+        <v>2.7</v>
       </c>
     </row>
     <row ht="27" r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" s="11344" t="s">
+      <c r="A22" s="11446" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="11394" t="n">
+      <c r="B22" s="11496" t="n">
         <v>0.67</v>
       </c>
     </row>
     <row ht="54" r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" s="11345" t="s">
+      <c r="A23" s="11447" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="11395" t="n">
+      <c r="B23" s="11497" t="n">
         <v>0.65</v>
       </c>
     </row>
     <row ht="27" r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24" s="11346" t="s">
+      <c r="A24" s="11448" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="11396" t="n">
+      <c r="B24" s="11498" t="n">
         <v>1.32</v>
       </c>
     </row>
     <row ht="67.5" r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" s="11347" t="s">
+      <c r="A25" s="11449" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="11397" t="n">
-        <v>0.73</v>
+      <c r="B25" s="11499" t="n">
+        <v>0.72</v>
       </c>
     </row>
     <row ht="40.5" r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" s="11348" t="s">
+      <c r="A26" s="11450" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="11398" t="n">
+      <c r="B26" s="11500" t="n">
         <v>0.39</v>
       </c>
     </row>
     <row ht="81" r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" s="11349" t="s">
+      <c r="A27" s="11451" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="11399" t="n">
+      <c r="B27" s="11501" t="n">
         <v>1.37</v>
       </c>
     </row>
     <row ht="54" r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="11350" t="s">
+      <c r="A28" s="11452" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="11400" t="n">
+      <c r="B28" s="11502" t="n">
         <v>1.56</v>
       </c>
     </row>
     <row ht="40.5" r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="11351" t="s">
+      <c r="A29" s="11453" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="11401" t="n">
-        <v>0.5</v>
+      <c r="B29" s="11503" t="n">
+        <v>0.52</v>
       </c>
     </row>
     <row ht="54" r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="11352" t="s">
+      <c r="A30" s="11454" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="11402" t="n">
-        <v>3.11</v>
+      <c r="B30" s="11504" t="n">
+        <v>3.07</v>
       </c>
     </row>
     <row ht="40.5" r="31" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A31" s="11353" t="s">
+      <c r="A31" s="11455" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="11403" t="n">
+      <c r="B31" s="11505" t="n">
         <v>10.61</v>
       </c>
     </row>
     <row ht="40.5" r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32" s="11354" t="s">
+      <c r="A32" s="11456" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="11404" t="n">
+      <c r="B32" s="11506" t="n">
         <v>1.32</v>
       </c>
     </row>
     <row ht="27" r="33" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A33" s="11355" t="s">
+      <c r="A33" s="11457" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="11405" t="n">
-        <v>1.93</v>
+      <c r="B33" s="11507" t="n">
+        <v>1.92</v>
       </c>
     </row>
     <row ht="67.5" r="34" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A34" s="11356" t="s">
+      <c r="A34" s="11458" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="11406" t="n">
+      <c r="B34" s="11508" t="n">
         <v>1.29</v>
       </c>
     </row>
     <row ht="54" r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35" s="11357" t="s">
+      <c r="A35" s="11459" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="11407" t="n">
-        <v>1.24</v>
+      <c r="B35" s="11509" t="n">
+        <v>1.27</v>
       </c>
     </row>
     <row ht="54" r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36" s="11358" t="s">
+      <c r="A36" s="11460" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="11408" t="n">
-        <v>1.39</v>
+      <c r="B36" s="11510" t="n">
+        <v>1.37</v>
       </c>
     </row>
     <row ht="40.5" r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37" s="11359" t="s">
+      <c r="A37" s="11461" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="11409" t="n">
-        <v>0.93</v>
+      <c r="B37" s="11511" t="n">
+        <v>0.91</v>
       </c>
     </row>
     <row ht="54" r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" s="11360" t="s">
+      <c r="A38" s="11462" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="11410" t="n">
-        <v>1.01</v>
+      <c r="B38" s="11512" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row ht="40.5" r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39" s="11361" t="s">
+      <c r="A39" s="11463" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="11411" t="n">
+      <c r="B39" s="11513" t="n">
         <v>1.7</v>
       </c>
     </row>
     <row ht="54" r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40" s="11362" t="s">
+      <c r="A40" s="11464" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="11412" t="n">
-        <v>6.28</v>
+      <c r="B40" s="11514" t="n">
+        <v>6.61</v>
       </c>
     </row>
     <row ht="54" r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41" s="11363" t="s">
+      <c r="A41" s="11465" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="11413" t="n">
-        <v>0.34</v>
+      <c r="B41" s="11515" t="n">
+        <v>0.33</v>
       </c>
     </row>
     <row ht="54" r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42" s="11364" t="s">
+      <c r="A42" s="11466" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="11414" t="n">
+      <c r="B42" s="11516" t="n">
         <v>0.44</v>
       </c>
     </row>
     <row ht="40.5" r="43" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A43" s="11365" t="s">
+      <c r="A43" s="11467" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="11415" t="n">
+      <c r="B43" s="11517" t="n">
         <v>1.05</v>
       </c>
     </row>
     <row ht="40.5" r="44" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A44" s="11366" t="s">
+      <c r="A44" s="11468" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="11416" t="n">
-        <v>1.57</v>
+      <c r="B44" s="11518" t="n">
+        <v>1.56</v>
       </c>
     </row>
     <row ht="54" r="45" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A45" s="11367" t="s">
+      <c r="A45" s="11469" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="11417" t="n">
+      <c r="B45" s="11519" t="n">
         <v>4.04</v>
       </c>
     </row>
     <row ht="81" r="46" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A46" s="11368" t="s">
+      <c r="A46" s="11470" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="11418" t="n">
-        <v>2.07</v>
+      <c r="B46" s="11520" t="n">
+        <v>2.05</v>
       </c>
     </row>
     <row ht="27" r="47" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A47" s="11369" t="s">
+      <c r="A47" s="11471" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="11419" t="n">
-        <v>2.26</v>
+      <c r="B47" s="11521" t="n">
+        <v>2.27</v>
       </c>
     </row>
     <row ht="54" r="48" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A48" s="11370" t="s">
+      <c r="A48" s="11472" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="11420" t="n">
-        <v>4.34</v>
+      <c r="B48" s="11522" t="n">
+        <v>4.35</v>
       </c>
     </row>
     <row ht="40.5" r="49" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A49" s="11371" t="s">
+      <c r="A49" s="11473" t="s">
         <v>46</v>
       </c>
-      <c r="B49" s="11421" t="n">
-        <v>2.06</v>
+      <c r="B49" s="11523" t="n">
+        <v>2.03</v>
       </c>
     </row>
     <row ht="54" r="50" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A50" s="11372" t="s">
+      <c r="A50" s="11474" t="s">
         <v>42</v>
       </c>
-      <c r="B50" s="11422" t="n">
-        <v>0.71</v>
+      <c r="B50" s="11524" t="n">
+        <v>0.7</v>
       </c>
     </row>
     <row ht="67.5" r="51" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A51" s="11373" t="s">
+      <c r="A51" s="11475" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="11423" t="n">
-        <v>1.1</v>
+      <c r="B51" s="11525" t="n">
+        <v>1.09</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
desktop 74 morning commit
</commit_message>
<xml_diff>
--- a/new.xlsx
+++ b/new.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5887" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5939" uniqueCount="74">
   <si>
     <t>stock</t>
   </si>
@@ -309,7 +309,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11730">
+  <cellXfs count="11832">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="176" xfId="5">
       <alignment wrapText="1"/>
@@ -20454,6 +20454,312 @@
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="176" xfId="5">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3">
@@ -35811,410 +36117,410 @@
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="11628" t="s">
+      <c r="A1" s="11730" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11629" t="s">
+      <c r="B1" s="11731" t="s">
         <v>1</v>
       </c>
     </row>
     <row ht="54" r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="11630" t="s">
+      <c r="A2" s="11732" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11680" t="n">
+      <c r="B2" s="11782" t="n">
         <v>2.87</v>
       </c>
     </row>
     <row ht="40.5" r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="11631" t="s">
+      <c r="A3" s="11733" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="11681" t="n">
+      <c r="B3" s="11783" t="n">
         <v>1.97</v>
       </c>
     </row>
     <row ht="27" r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="11632" t="s">
+      <c r="A4" s="11734" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="11682" t="n">
+      <c r="B4" s="11784" t="n">
         <v>2.62</v>
       </c>
     </row>
     <row ht="27" r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="11633" t="s">
+      <c r="A5" s="11735" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="11683" t="n">
+      <c r="B5" s="11785" t="n">
         <v>2.29</v>
       </c>
     </row>
     <row ht="40.5" r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="11634" t="s">
+      <c r="A6" s="11736" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="11684" t="n">
+      <c r="B6" s="11786" t="n">
         <v>1.31</v>
       </c>
     </row>
     <row ht="67.5" r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="11635" t="s">
+      <c r="A7" s="11737" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="11685" t="n">
+      <c r="B7" s="11787" t="n">
         <v>5.4</v>
       </c>
     </row>
     <row ht="27" r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" s="11636" t="s">
+      <c r="A8" s="11738" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="11686" t="n">
+      <c r="B8" s="11788" t="n">
         <v>1.8</v>
       </c>
     </row>
     <row ht="54" r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" s="11637" t="s">
+      <c r="A9" s="11739" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="11687" t="n">
+      <c r="B9" s="11789" t="n">
         <v>1.06</v>
       </c>
     </row>
     <row ht="27" r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" s="11638" t="s">
+      <c r="A10" s="11740" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="11688" t="n">
+      <c r="B10" s="11790" t="n">
         <v>1.41</v>
       </c>
     </row>
     <row ht="40.5" r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" s="11639" t="s">
+      <c r="A11" s="11741" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="11689" t="n">
+      <c r="B11" s="11791" t="n">
         <v>2.85</v>
       </c>
     </row>
     <row ht="81" r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" s="11640" t="s">
+      <c r="A12" s="11742" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="11690" t="n">
+      <c r="B12" s="11792" t="n">
         <v>1.03</v>
       </c>
     </row>
     <row ht="27" r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" s="11641" t="s">
+      <c r="A13" s="11743" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="11691" t="n">
+      <c r="B13" s="11793" t="n">
         <v>0.89</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" s="11642" t="s">
+      <c r="A14" s="11744" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="11692" t="n">
+      <c r="B14" s="11794" t="n">
         <v>0.35</v>
       </c>
     </row>
     <row ht="40.5" r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" s="11643" t="s">
+      <c r="A15" s="11745" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="11693" t="n">
+      <c r="B15" s="11795" t="n">
         <v>1.02</v>
       </c>
     </row>
     <row ht="67.5" r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" s="11644" t="s">
+      <c r="A16" s="11746" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="11694" t="n">
+      <c r="B16" s="11796" t="n">
         <v>4.83</v>
       </c>
     </row>
     <row ht="40.5" r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" s="11645" t="s">
+      <c r="A17" s="11747" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="11695" t="n">
+      <c r="B17" s="11797" t="n">
         <v>0.81</v>
       </c>
     </row>
     <row ht="40.5" r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" s="11646" t="s">
+      <c r="A18" s="11748" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="11696" t="n">
+      <c r="B18" s="11798" t="n">
         <v>1.27</v>
       </c>
     </row>
     <row ht="27" r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" s="11647" t="s">
+      <c r="A19" s="11749" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="11697" t="n">
+      <c r="B19" s="11799" t="n">
         <v>3.52</v>
       </c>
     </row>
     <row ht="67.5" r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" s="11648" t="s">
+      <c r="A20" s="11750" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="11698" t="n">
+      <c r="B20" s="11800" t="n">
         <v>1.99</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" s="11649" t="s">
+      <c r="A21" s="11751" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="11699" t="n">
+      <c r="B21" s="11801" t="n">
         <v>2.69</v>
       </c>
     </row>
     <row ht="27" r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" s="11650" t="s">
+      <c r="A22" s="11752" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="11700" t="n">
+      <c r="B22" s="11802" t="n">
         <v>0.67</v>
       </c>
     </row>
     <row ht="54" r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" s="11651" t="s">
+      <c r="A23" s="11753" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="11701" t="n">
+      <c r="B23" s="11803" t="n">
         <v>0.63</v>
       </c>
     </row>
     <row ht="27" r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24" s="11652" t="s">
+      <c r="A24" s="11754" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="11702" t="n">
+      <c r="B24" s="11804" t="n">
         <v>1.32</v>
       </c>
     </row>
     <row ht="67.5" r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" s="11653" t="s">
+      <c r="A25" s="11755" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="11703" t="n">
+      <c r="B25" s="11805" t="n">
         <v>0.72</v>
       </c>
     </row>
     <row ht="40.5" r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" s="11654" t="s">
+      <c r="A26" s="11756" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="11704" t="n">
+      <c r="B26" s="11806" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row ht="81" r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" s="11655" t="s">
+      <c r="A27" s="11757" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="11705" t="n">
+      <c r="B27" s="11807" t="n">
         <v>1.41</v>
       </c>
     </row>
     <row ht="54" r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="11656" t="s">
+      <c r="A28" s="11758" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="11706" t="n">
+      <c r="B28" s="11808" t="n">
         <v>1.57</v>
       </c>
     </row>
     <row ht="40.5" r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="11657" t="s">
+      <c r="A29" s="11759" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="11707" t="n">
+      <c r="B29" s="11809" t="n">
         <v>0.52</v>
       </c>
     </row>
     <row ht="54" r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="11658" t="s">
+      <c r="A30" s="11760" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="11708" t="n">
+      <c r="B30" s="11810" t="n">
         <v>3.06</v>
       </c>
     </row>
     <row ht="40.5" r="31" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A31" s="11659" t="s">
+      <c r="A31" s="11761" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="11709" t="n">
+      <c r="B31" s="11811" t="n">
         <v>10.57</v>
       </c>
     </row>
     <row ht="40.5" r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32" s="11660" t="s">
+      <c r="A32" s="11762" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="11710" t="n">
+      <c r="B32" s="11812" t="n">
         <v>1.28</v>
       </c>
     </row>
     <row ht="27" r="33" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A33" s="11661" t="s">
+      <c r="A33" s="11763" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="11711" t="n">
+      <c r="B33" s="11813" t="n">
         <v>1.94</v>
       </c>
     </row>
     <row ht="67.5" r="34" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A34" s="11662" t="s">
+      <c r="A34" s="11764" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="11712" t="n">
+      <c r="B34" s="11814" t="n">
         <v>1.31</v>
       </c>
     </row>
     <row ht="54" r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35" s="11663" t="s">
+      <c r="A35" s="11765" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="11713" t="n">
+      <c r="B35" s="11815" t="n">
         <v>1.27</v>
       </c>
     </row>
     <row ht="54" r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36" s="11664" t="s">
+      <c r="A36" s="11766" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="11714" t="n">
+      <c r="B36" s="11816" t="n">
         <v>1.35</v>
       </c>
     </row>
     <row ht="40.5" r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37" s="11665" t="s">
+      <c r="A37" s="11767" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="11715" t="n">
+      <c r="B37" s="11817" t="n">
         <v>0.91</v>
       </c>
     </row>
     <row ht="54" r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" s="11666" t="s">
+      <c r="A38" s="11768" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="11716" t="n">
+      <c r="B38" s="11818" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row ht="40.5" r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39" s="11667" t="s">
+      <c r="A39" s="11769" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="11717" t="n">
+      <c r="B39" s="11819" t="n">
         <v>1.69</v>
       </c>
     </row>
     <row ht="54" r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40" s="11668" t="s">
+      <c r="A40" s="11770" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="11718" t="n">
+      <c r="B40" s="11820" t="n">
         <v>6.51</v>
       </c>
     </row>
     <row ht="54" r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41" s="11669" t="s">
+      <c r="A41" s="11771" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="11719" t="n">
+      <c r="B41" s="11821" t="n">
         <v>0.32</v>
       </c>
     </row>
     <row ht="54" r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42" s="11670" t="s">
+      <c r="A42" s="11772" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="11720" t="n">
+      <c r="B42" s="11822" t="n">
         <v>0.44</v>
       </c>
     </row>
     <row ht="40.5" r="43" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A43" s="11671" t="s">
+      <c r="A43" s="11773" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="11721" t="n">
+      <c r="B43" s="11823" t="n">
         <v>1.02</v>
       </c>
     </row>
     <row ht="40.5" r="44" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A44" s="11672" t="s">
+      <c r="A44" s="11774" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="11722" t="n">
+      <c r="B44" s="11824" t="n">
         <v>1.57</v>
       </c>
     </row>
     <row ht="54" r="45" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A45" s="11673" t="s">
+      <c r="A45" s="11775" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="11723" t="n">
+      <c r="B45" s="11825" t="n">
         <v>4.03</v>
       </c>
     </row>
     <row ht="81" r="46" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A46" s="11674" t="s">
+      <c r="A46" s="11776" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="11724" t="n">
+      <c r="B46" s="11826" t="n">
         <v>2.06</v>
       </c>
     </row>
     <row ht="27" r="47" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A47" s="11675" t="s">
+      <c r="A47" s="11777" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="11725" t="n">
+      <c r="B47" s="11827" t="n">
         <v>2.22</v>
       </c>
     </row>
     <row ht="54" r="48" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A48" s="11676" t="s">
+      <c r="A48" s="11778" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="11726" t="n">
+      <c r="B48" s="11828" t="n">
         <v>4.38</v>
       </c>
     </row>
     <row ht="40.5" r="49" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A49" s="11677" t="s">
+      <c r="A49" s="11779" t="s">
         <v>46</v>
       </c>
-      <c r="B49" s="11727" t="n">
+      <c r="B49" s="11829" t="n">
         <v>2.07</v>
       </c>
     </row>
     <row ht="54" r="50" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A50" s="11678" t="s">
+      <c r="A50" s="11780" t="s">
         <v>42</v>
       </c>
-      <c r="B50" s="11728" t="n">
+      <c r="B50" s="11830" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row ht="67.5" r="51" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A51" s="11679" t="s">
+      <c r="A51" s="11781" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="11729" t="n">
+      <c r="B51" s="11831" t="n">
         <v>1.08</v>
       </c>
     </row>

</xml_diff>